<commit_message>
added data and dna samples
</commit_message>
<xml_diff>
--- a/data/master_sample_manifest.xlsx
+++ b/data/master_sample_manifest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/moorea_symbiotic_exchange_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369B64B5-A1E2-D140-9DC5-1156FC0AFF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0E3543-9DAE-4449-B9AF-CBA169C8A07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12840" yWindow="820" windowWidth="17180" windowHeight="17560" xr2:uid="{6B87E6CE-126B-8B47-B516-351EEAF1A0B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="159">
   <si>
     <t>sample_id</t>
   </si>
@@ -53,141 +53,6 @@
     <t>experiment</t>
   </si>
   <si>
-    <t>ACR-A-1</t>
-  </si>
-  <si>
-    <t>ACR-A-2</t>
-  </si>
-  <si>
-    <t>ACR-A-3</t>
-  </si>
-  <si>
-    <t>ACR-A-4</t>
-  </si>
-  <si>
-    <t>ACR-A-5</t>
-  </si>
-  <si>
-    <t>ACR-R-1</t>
-  </si>
-  <si>
-    <t>ACR-R-2</t>
-  </si>
-  <si>
-    <t>ACR-R-3</t>
-  </si>
-  <si>
-    <t>ACR-R-4</t>
-  </si>
-  <si>
-    <t>ACR-R-5</t>
-  </si>
-  <si>
-    <t>ACR-R-6</t>
-  </si>
-  <si>
-    <t>ACR-R-7</t>
-  </si>
-  <si>
-    <t>ACR-R-8</t>
-  </si>
-  <si>
-    <t>ACR-R-9</t>
-  </si>
-  <si>
-    <t>ACR-R-10</t>
-  </si>
-  <si>
-    <t>POC-A-1</t>
-  </si>
-  <si>
-    <t>POC-A-2</t>
-  </si>
-  <si>
-    <t>POC-A-3</t>
-  </si>
-  <si>
-    <t>POC-A-4</t>
-  </si>
-  <si>
-    <t>POC-A-5</t>
-  </si>
-  <si>
-    <t>POC-R-1</t>
-  </si>
-  <si>
-    <t>POC-R-2</t>
-  </si>
-  <si>
-    <t>POC-R-3</t>
-  </si>
-  <si>
-    <t>POC-R-4</t>
-  </si>
-  <si>
-    <t>POC-R-5</t>
-  </si>
-  <si>
-    <t>POC-R-6</t>
-  </si>
-  <si>
-    <t>POC-R-7</t>
-  </si>
-  <si>
-    <t>POC-R-8</t>
-  </si>
-  <si>
-    <t>POC-R-9</t>
-  </si>
-  <si>
-    <t>POC-R-10</t>
-  </si>
-  <si>
-    <t>POR-A-1</t>
-  </si>
-  <si>
-    <t>POR-A-2</t>
-  </si>
-  <si>
-    <t>POR-A-3</t>
-  </si>
-  <si>
-    <t>POR-A-4</t>
-  </si>
-  <si>
-    <t>POR-A-5</t>
-  </si>
-  <si>
-    <t>POR-R-1</t>
-  </si>
-  <si>
-    <t>POR-R-2</t>
-  </si>
-  <si>
-    <t>POR-R-3</t>
-  </si>
-  <si>
-    <t>POR-R-4</t>
-  </si>
-  <si>
-    <t>POR-R-5</t>
-  </si>
-  <si>
-    <t>POR-R-6</t>
-  </si>
-  <si>
-    <t>POR-R-7</t>
-  </si>
-  <si>
-    <t>POR-R-8</t>
-  </si>
-  <si>
-    <t>POR-R-9</t>
-  </si>
-  <si>
-    <t>POR-R-10</t>
-  </si>
-  <si>
     <t>Acropora</t>
   </si>
   <si>
@@ -206,307 +71,448 @@
     <t>PI Curves</t>
   </si>
   <si>
-    <t>ACR-A-6</t>
-  </si>
-  <si>
-    <t>ACR-A-7</t>
-  </si>
-  <si>
-    <t>ACR-A-8</t>
-  </si>
-  <si>
-    <t>ACR-A-9</t>
-  </si>
-  <si>
-    <t>ACR-A-10</t>
-  </si>
-  <si>
-    <t>ACR-A-11</t>
-  </si>
-  <si>
-    <t>ACR-A-12</t>
-  </si>
-  <si>
-    <t>ACR-A-13</t>
-  </si>
-  <si>
-    <t>ACR-A-14</t>
-  </si>
-  <si>
-    <t>ACR-A-15</t>
-  </si>
-  <si>
-    <t>ACR-A-16</t>
-  </si>
-  <si>
-    <t>ACR-A-17</t>
-  </si>
-  <si>
-    <t>ACR-R-11</t>
-  </si>
-  <si>
-    <t>ACR-R-12</t>
-  </si>
-  <si>
-    <t>ACR-R-13</t>
-  </si>
-  <si>
-    <t>ACR-R-14</t>
-  </si>
-  <si>
-    <t>ACR-R-15</t>
-  </si>
-  <si>
-    <t>ACR-R-16</t>
-  </si>
-  <si>
-    <t>ACR-R-17</t>
-  </si>
-  <si>
-    <t>ACR-R-18</t>
-  </si>
-  <si>
-    <t>ACR-R-19</t>
-  </si>
-  <si>
-    <t>ACR-R-20</t>
-  </si>
-  <si>
-    <t>ACR-R-21</t>
-  </si>
-  <si>
-    <t>ACR-R-22</t>
-  </si>
-  <si>
-    <t>ACR-R-23</t>
-  </si>
-  <si>
-    <t>ACR-R-24</t>
-  </si>
-  <si>
-    <t>ACR-R-25</t>
-  </si>
-  <si>
-    <t>ACR-R-26</t>
-  </si>
-  <si>
-    <t>ACR-R-27</t>
-  </si>
-  <si>
-    <t>ACR-R-28</t>
-  </si>
-  <si>
-    <t>ACR-R-29</t>
-  </si>
-  <si>
-    <t>ACR-R-30</t>
-  </si>
-  <si>
-    <t>POC-A-6</t>
-  </si>
-  <si>
-    <t>POC-A-7</t>
-  </si>
-  <si>
-    <t>POC-A-8</t>
-  </si>
-  <si>
-    <t>POC-A-9</t>
-  </si>
-  <si>
-    <t>POC-A-10</t>
-  </si>
-  <si>
-    <t>POC-A-11</t>
-  </si>
-  <si>
-    <t>POC-A-12</t>
-  </si>
-  <si>
-    <t>POC-A-13</t>
-  </si>
-  <si>
-    <t>POC-A-14</t>
-  </si>
-  <si>
-    <t>POC-A-15</t>
-  </si>
-  <si>
-    <t>POC-A-16</t>
-  </si>
-  <si>
-    <t>POC-A-17</t>
-  </si>
-  <si>
-    <t>POC-R-11</t>
-  </si>
-  <si>
-    <t>POC-R-12</t>
-  </si>
-  <si>
-    <t>POC-R-13</t>
-  </si>
-  <si>
-    <t>POC-R-14</t>
-  </si>
-  <si>
-    <t>POC-R-15</t>
-  </si>
-  <si>
-    <t>POC-R-16</t>
-  </si>
-  <si>
-    <t>POC-R-17</t>
-  </si>
-  <si>
-    <t>POC-R-18</t>
-  </si>
-  <si>
-    <t>POC-R-19</t>
-  </si>
-  <si>
-    <t>POC-R-20</t>
-  </si>
-  <si>
-    <t>POC-R-21</t>
-  </si>
-  <si>
-    <t>POC-R-22</t>
-  </si>
-  <si>
-    <t>POC-R-23</t>
-  </si>
-  <si>
-    <t>POC-R-24</t>
-  </si>
-  <si>
-    <t>POC-R-25</t>
-  </si>
-  <si>
-    <t>POC-R-26</t>
-  </si>
-  <si>
-    <t>POC-R-27</t>
-  </si>
-  <si>
-    <t>POC-R-28</t>
-  </si>
-  <si>
-    <t>POC-R-29</t>
-  </si>
-  <si>
-    <t>POC-R-30</t>
-  </si>
-  <si>
-    <t>POR-A-6</t>
-  </si>
-  <si>
-    <t>POR-A-7</t>
-  </si>
-  <si>
-    <t>POR-A-8</t>
-  </si>
-  <si>
-    <t>POR-A-9</t>
-  </si>
-  <si>
-    <t>POR-A-10</t>
-  </si>
-  <si>
-    <t>POR-A-11</t>
-  </si>
-  <si>
-    <t>POR-A-12</t>
-  </si>
-  <si>
-    <t>POR-A-13</t>
-  </si>
-  <si>
-    <t>POR-A-14</t>
-  </si>
-  <si>
-    <t>POR-A-15</t>
-  </si>
-  <si>
-    <t>POR-A-16</t>
-  </si>
-  <si>
-    <t>POR-A-17</t>
-  </si>
-  <si>
-    <t>POR-R-11</t>
-  </si>
-  <si>
-    <t>POR-R-12</t>
-  </si>
-  <si>
-    <t>POR-R-13</t>
-  </si>
-  <si>
-    <t>POR-R-14</t>
-  </si>
-  <si>
-    <t>POR-R-15</t>
-  </si>
-  <si>
-    <t>POR-R-16</t>
-  </si>
-  <si>
-    <t>POR-R-17</t>
-  </si>
-  <si>
-    <t>POR-R-18</t>
-  </si>
-  <si>
-    <t>POR-R-19</t>
-  </si>
-  <si>
-    <t>POR-R-20</t>
-  </si>
-  <si>
-    <t>POR-R-21</t>
-  </si>
-  <si>
-    <t>POR-R-22</t>
-  </si>
-  <si>
-    <t>POR-R-23</t>
-  </si>
-  <si>
-    <t>POR-R-24</t>
-  </si>
-  <si>
-    <t>POR-R-25</t>
-  </si>
-  <si>
-    <t>POR-R-26</t>
-  </si>
-  <si>
-    <t>POR-R-27</t>
-  </si>
-  <si>
-    <t>POR-R-28</t>
-  </si>
-  <si>
-    <t>POR-R-29</t>
-  </si>
-  <si>
-    <t>POR-R-30</t>
-  </si>
-  <si>
     <t>dna.tube</t>
   </si>
   <si>
-    <t>rna.tube</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>PR Rates</t>
   </si>
   <si>
-    <t>whirlpack</t>
+    <t>dna.location</t>
+  </si>
+  <si>
+    <t>whirlpack.location</t>
+  </si>
+  <si>
+    <t>airbrushed</t>
+  </si>
+  <si>
+    <t>slurry.location</t>
+  </si>
+  <si>
+    <t>ACR-A1</t>
+  </si>
+  <si>
+    <t>ACR-A2</t>
+  </si>
+  <si>
+    <t>ACR-A3</t>
+  </si>
+  <si>
+    <t>ACR-A4</t>
+  </si>
+  <si>
+    <t>ACR-A5</t>
+  </si>
+  <si>
+    <t>ACR-R1</t>
+  </si>
+  <si>
+    <t>ACR-R2</t>
+  </si>
+  <si>
+    <t>ACR-R3</t>
+  </si>
+  <si>
+    <t>ACR-R4</t>
+  </si>
+  <si>
+    <t>ACR-R5</t>
+  </si>
+  <si>
+    <t>ACR-R6</t>
+  </si>
+  <si>
+    <t>ACR-R7</t>
+  </si>
+  <si>
+    <t>ACR-R8</t>
+  </si>
+  <si>
+    <t>ACR-R9</t>
+  </si>
+  <si>
+    <t>ACR-R10</t>
+  </si>
+  <si>
+    <t>POC-A1</t>
+  </si>
+  <si>
+    <t>POC-A2</t>
+  </si>
+  <si>
+    <t>POC-A3</t>
+  </si>
+  <si>
+    <t>POC-A4</t>
+  </si>
+  <si>
+    <t>POC-A5</t>
+  </si>
+  <si>
+    <t>POC-R1</t>
+  </si>
+  <si>
+    <t>POC-R2</t>
+  </si>
+  <si>
+    <t>POC-R3</t>
+  </si>
+  <si>
+    <t>POC-R4</t>
+  </si>
+  <si>
+    <t>POC-R5</t>
+  </si>
+  <si>
+    <t>POC-R6</t>
+  </si>
+  <si>
+    <t>POC-R7</t>
+  </si>
+  <si>
+    <t>POC-R8</t>
+  </si>
+  <si>
+    <t>POC-R9</t>
+  </si>
+  <si>
+    <t>POC-R10</t>
+  </si>
+  <si>
+    <t>POR-A1</t>
+  </si>
+  <si>
+    <t>POR-A2</t>
+  </si>
+  <si>
+    <t>POR-A3</t>
+  </si>
+  <si>
+    <t>POR-A4</t>
+  </si>
+  <si>
+    <t>POR-A5</t>
+  </si>
+  <si>
+    <t>POR-R1</t>
+  </si>
+  <si>
+    <t>POR-R2</t>
+  </si>
+  <si>
+    <t>POR-R3</t>
+  </si>
+  <si>
+    <t>POR-R4</t>
+  </si>
+  <si>
+    <t>POR-R5</t>
+  </si>
+  <si>
+    <t>POR-R6</t>
+  </si>
+  <si>
+    <t>POR-R7</t>
+  </si>
+  <si>
+    <t>POR-R8</t>
+  </si>
+  <si>
+    <t>POR-R9</t>
+  </si>
+  <si>
+    <t>POR-R10</t>
+  </si>
+  <si>
+    <t>ACR-A6</t>
+  </si>
+  <si>
+    <t>ACR-A7</t>
+  </si>
+  <si>
+    <t>ACR-A8</t>
+  </si>
+  <si>
+    <t>ACR-A9</t>
+  </si>
+  <si>
+    <t>ACR-A10</t>
+  </si>
+  <si>
+    <t>ACR-A11</t>
+  </si>
+  <si>
+    <t>ACR-A12</t>
+  </si>
+  <si>
+    <t>ACR-A13</t>
+  </si>
+  <si>
+    <t>ACR-A14</t>
+  </si>
+  <si>
+    <t>ACR-A15</t>
+  </si>
+  <si>
+    <t>ACR-A16</t>
+  </si>
+  <si>
+    <t>ACR-A17</t>
+  </si>
+  <si>
+    <t>ACR-R11</t>
+  </si>
+  <si>
+    <t>ACR-R13</t>
+  </si>
+  <si>
+    <t>ACR-R12</t>
+  </si>
+  <si>
+    <t>ACR-R14</t>
+  </si>
+  <si>
+    <t>ACR-R15</t>
+  </si>
+  <si>
+    <t>ACR-R16</t>
+  </si>
+  <si>
+    <t>ACR-R17</t>
+  </si>
+  <si>
+    <t>ACR-R18</t>
+  </si>
+  <si>
+    <t>ACR-R19</t>
+  </si>
+  <si>
+    <t>ACR-R20</t>
+  </si>
+  <si>
+    <t>ACR-R21</t>
+  </si>
+  <si>
+    <t>ACR-R22</t>
+  </si>
+  <si>
+    <t>ACR-R23</t>
+  </si>
+  <si>
+    <t>ACR-R24</t>
+  </si>
+  <si>
+    <t>ACR-R25</t>
+  </si>
+  <si>
+    <t>ACR-R26</t>
+  </si>
+  <si>
+    <t>ACR-R27</t>
+  </si>
+  <si>
+    <t>ACR-R28</t>
+  </si>
+  <si>
+    <t>ACR-R29</t>
+  </si>
+  <si>
+    <t>ACR-R30</t>
+  </si>
+  <si>
+    <t>POC-A6</t>
+  </si>
+  <si>
+    <t>POC-A7</t>
+  </si>
+  <si>
+    <t>POC-A8</t>
+  </si>
+  <si>
+    <t>POC-A9</t>
+  </si>
+  <si>
+    <t>POC-A10</t>
+  </si>
+  <si>
+    <t>POC-A11</t>
+  </si>
+  <si>
+    <t>POC-A12</t>
+  </si>
+  <si>
+    <t>POC-A13</t>
+  </si>
+  <si>
+    <t>POC-A14</t>
+  </si>
+  <si>
+    <t>POC-A15</t>
+  </si>
+  <si>
+    <t>POC-A16</t>
+  </si>
+  <si>
+    <t>POC-A17</t>
+  </si>
+  <si>
+    <t>POC-R11</t>
+  </si>
+  <si>
+    <t>POC-R12</t>
+  </si>
+  <si>
+    <t>POC-R13</t>
+  </si>
+  <si>
+    <t>POC-R14</t>
+  </si>
+  <si>
+    <t>POC-R15</t>
+  </si>
+  <si>
+    <t>POC-R16</t>
+  </si>
+  <si>
+    <t>POC-R17</t>
+  </si>
+  <si>
+    <t>POC-R18</t>
+  </si>
+  <si>
+    <t>POC-R19</t>
+  </si>
+  <si>
+    <t>POC-R20</t>
+  </si>
+  <si>
+    <t>POC-R21</t>
+  </si>
+  <si>
+    <t>POC-R22</t>
+  </si>
+  <si>
+    <t>POC-R23</t>
+  </si>
+  <si>
+    <t>POC-R24</t>
+  </si>
+  <si>
+    <t>POC-R25</t>
+  </si>
+  <si>
+    <t>POC-R26</t>
+  </si>
+  <si>
+    <t>POC-R27</t>
+  </si>
+  <si>
+    <t>POC-R28</t>
+  </si>
+  <si>
+    <t>POC-R29</t>
+  </si>
+  <si>
+    <t>POC-R30</t>
+  </si>
+  <si>
+    <t>POR-A6</t>
+  </si>
+  <si>
+    <t>POR-A7</t>
+  </si>
+  <si>
+    <t>POR-A8</t>
+  </si>
+  <si>
+    <t>POR-A9</t>
+  </si>
+  <si>
+    <t>POR-A10</t>
+  </si>
+  <si>
+    <t>POR-A11</t>
+  </si>
+  <si>
+    <t>POR-A12</t>
+  </si>
+  <si>
+    <t>POR-A13</t>
+  </si>
+  <si>
+    <t>POR-A14</t>
+  </si>
+  <si>
+    <t>POR-A15</t>
+  </si>
+  <si>
+    <t>POR-A16</t>
+  </si>
+  <si>
+    <t>POR-A17</t>
+  </si>
+  <si>
+    <t>POR-R11</t>
+  </si>
+  <si>
+    <t>POR-R12</t>
+  </si>
+  <si>
+    <t>POR-R13</t>
+  </si>
+  <si>
+    <t>POR-R14</t>
+  </si>
+  <si>
+    <t>POR-R15</t>
+  </si>
+  <si>
+    <t>POR-R16</t>
+  </si>
+  <si>
+    <t>POR-R17</t>
+  </si>
+  <si>
+    <t>POR-R18</t>
+  </si>
+  <si>
+    <t>POR-R19</t>
+  </si>
+  <si>
+    <t>POR-R20</t>
+  </si>
+  <si>
+    <t>POR-R21</t>
+  </si>
+  <si>
+    <t>POR-R22</t>
+  </si>
+  <si>
+    <t>POR-R23</t>
+  </si>
+  <si>
+    <t>POR-R24</t>
+  </si>
+  <si>
+    <t>POR-R25</t>
+  </si>
+  <si>
+    <t>POR-R26</t>
+  </si>
+  <si>
+    <t>POR-R27</t>
+  </si>
+  <si>
+    <t>POR-R28</t>
+  </si>
+  <si>
+    <t>POR-R29</t>
+  </si>
+  <si>
+    <t>POR-R30</t>
+  </si>
+  <si>
+    <t>Molecular -40</t>
   </si>
 </sst>
 </file>
@@ -871,24 +877,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5716CA15-A063-CD4A-965E-FFCB3C4243EA}">
-  <dimension ref="A1:K142"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,2683 +911,2686 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>20231104</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>20231104</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>20231104</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>20231104</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>20231104</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>20231104</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>102</v>
       </c>
       <c r="G7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>20231104</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>20231104</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>104</v>
       </c>
       <c r="G9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>20231104</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>105</v>
       </c>
       <c r="G10" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>20231104</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D12">
         <v>20231104</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>107</v>
       </c>
       <c r="G12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>20231104</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>108</v>
       </c>
       <c r="G13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>20231104</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>109</v>
       </c>
       <c r="G14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D15">
         <v>20231104</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D16">
         <v>20231104</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>20231104</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>112</v>
       </c>
       <c r="G17" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>20231104</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>113</v>
       </c>
       <c r="G18" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D19">
         <v>20231104</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>114</v>
       </c>
       <c r="G19" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D20">
         <v>20231104</v>
       </c>
       <c r="E20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>115</v>
       </c>
       <c r="G20" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>20231104</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>116</v>
       </c>
       <c r="G21" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>20231104</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>117</v>
       </c>
       <c r="G22" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>20231104</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>118</v>
       </c>
       <c r="G23" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <v>20231104</v>
       </c>
       <c r="E24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>119</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D25">
         <v>20231104</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>120</v>
       </c>
       <c r="G25" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <v>20231104</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>121</v>
       </c>
       <c r="G26" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D27">
         <v>20231104</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D28">
         <v>20231104</v>
       </c>
       <c r="E28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>123</v>
       </c>
       <c r="G28" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>20231104</v>
       </c>
       <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>139</v>
       </c>
       <c r="G29" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D30">
         <v>20231104</v>
       </c>
       <c r="E30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>125</v>
       </c>
       <c r="G30" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>20231104</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>126</v>
       </c>
       <c r="G31" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D32">
         <v>20231104</v>
       </c>
       <c r="E32" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>127</v>
       </c>
       <c r="G32" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D33">
         <v>20231104</v>
       </c>
       <c r="E33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>128</v>
       </c>
       <c r="G33" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D34">
         <v>20231104</v>
       </c>
       <c r="E34" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>129</v>
       </c>
       <c r="G34" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>20231104</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>130</v>
       </c>
       <c r="G35" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>20231104</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>131</v>
       </c>
       <c r="G36" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D37">
         <v>20231104</v>
       </c>
       <c r="E37" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>132</v>
       </c>
       <c r="G37" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D38">
         <v>20231104</v>
       </c>
       <c r="E38" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>133</v>
       </c>
       <c r="G38" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D39">
         <v>20231104</v>
       </c>
       <c r="E39" t="s">
-        <v>55</v>
-      </c>
-      <c r="F39" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>134</v>
       </c>
       <c r="G39" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D40">
         <v>20231104</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F40">
+        <v>135</v>
       </c>
       <c r="G40" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D41">
         <v>20231104</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>136</v>
       </c>
       <c r="G41" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D42">
         <v>20231104</v>
       </c>
       <c r="E42" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F42">
+        <v>137</v>
       </c>
       <c r="G42" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D43">
         <v>20231104</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>138</v>
       </c>
       <c r="G43" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D44">
         <v>20231104</v>
       </c>
       <c r="E44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F44">
+        <v>124</v>
       </c>
       <c r="G44" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D45">
         <v>20231104</v>
       </c>
       <c r="E45" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>140</v>
       </c>
       <c r="G45" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D46">
         <v>20231104</v>
       </c>
       <c r="E46" t="s">
-        <v>55</v>
-      </c>
-      <c r="F46" t="s">
-        <v>154</v>
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>141</v>
       </c>
       <c r="G46" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D47">
         <v>20231106</v>
       </c>
       <c r="E47" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D48">
         <v>20231106</v>
       </c>
       <c r="E48" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D49">
         <v>20231106</v>
       </c>
       <c r="E49" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D50">
         <v>20231106</v>
       </c>
       <c r="E50" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D51">
         <v>20231106</v>
       </c>
       <c r="E51" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D52">
         <v>20231106</v>
       </c>
       <c r="E52" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D53">
         <v>20231106</v>
       </c>
       <c r="E53" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D54">
         <v>20231106</v>
       </c>
       <c r="E54" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D55">
         <v>20231106</v>
       </c>
       <c r="E55" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D56">
         <v>20231106</v>
       </c>
       <c r="E56" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D57">
         <v>20231106</v>
       </c>
       <c r="E57" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D58">
         <v>20231106</v>
       </c>
       <c r="E58" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D59">
         <v>20231106</v>
       </c>
       <c r="E59" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D60">
         <v>20231106</v>
       </c>
       <c r="E60" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D61">
         <v>20231106</v>
       </c>
       <c r="E61" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D62">
         <v>20231106</v>
       </c>
       <c r="E62" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D63">
         <v>20231106</v>
       </c>
       <c r="E63" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D64">
         <v>20231106</v>
       </c>
       <c r="E64" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D65">
         <v>20231106</v>
       </c>
       <c r="E65" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D66">
         <v>20231106</v>
       </c>
       <c r="E66" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D67">
         <v>20231106</v>
       </c>
       <c r="E67" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D68">
         <v>20231106</v>
       </c>
       <c r="E68" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D69">
         <v>20231106</v>
       </c>
       <c r="E69" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D70">
         <v>20231106</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D71">
         <v>20231106</v>
       </c>
       <c r="E71" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D72">
         <v>20231106</v>
       </c>
       <c r="E72" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D73">
         <v>20231106</v>
       </c>
       <c r="E73" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D74">
         <v>20231106</v>
       </c>
       <c r="E74" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D75">
         <v>20231106</v>
       </c>
       <c r="E75" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D76">
         <v>20231106</v>
       </c>
       <c r="E76" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D77">
         <v>20231106</v>
       </c>
       <c r="E77" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D78">
         <v>20231106</v>
       </c>
       <c r="E78" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B79" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D79">
         <v>20231106</v>
       </c>
       <c r="E79" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B80" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D80">
         <v>20231106</v>
       </c>
       <c r="E80" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D81">
         <v>20231106</v>
       </c>
       <c r="E81" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D82">
         <v>20231106</v>
       </c>
       <c r="E82" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D83">
         <v>20231106</v>
       </c>
       <c r="E83" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B84" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D84">
         <v>20231106</v>
       </c>
       <c r="E84" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B85" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D85">
         <v>20231106</v>
       </c>
       <c r="E85" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D86">
         <v>20231106</v>
       </c>
       <c r="E86" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D87">
         <v>20231106</v>
       </c>
       <c r="E87" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B88" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D88">
         <v>20231106</v>
       </c>
       <c r="E88" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B89" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D89">
         <v>20231106</v>
       </c>
       <c r="E89" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B90" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D90">
         <v>20231106</v>
       </c>
       <c r="E90" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B91" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C91" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D91">
         <v>20231106</v>
       </c>
       <c r="E91" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D92">
         <v>20231106</v>
       </c>
       <c r="E92" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D93">
         <v>20231106</v>
       </c>
       <c r="E93" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D94">
         <v>20231106</v>
       </c>
       <c r="E94" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B95" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D95">
         <v>20231106</v>
       </c>
       <c r="E95" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B96" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D96">
         <v>20231106</v>
       </c>
       <c r="E96" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D97">
         <v>20231106</v>
       </c>
       <c r="E97" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B98" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D98">
         <v>20231106</v>
       </c>
       <c r="E98" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D99">
         <v>20231106</v>
       </c>
       <c r="E99" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B100" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D100">
         <v>20231106</v>
       </c>
       <c r="E100" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B101" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D101">
         <v>20231106</v>
       </c>
       <c r="E101" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B102" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D102">
         <v>20231106</v>
       </c>
       <c r="E102" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B103" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D103">
         <v>20231106</v>
       </c>
       <c r="E103" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B104" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D104">
         <v>20231106</v>
       </c>
       <c r="E104" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B105" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D105">
         <v>20231106</v>
       </c>
       <c r="E105" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B106" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D106">
         <v>20231106</v>
       </c>
       <c r="E106" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B107" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D107">
         <v>20231106</v>
       </c>
       <c r="E107" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D108">
         <v>20231106</v>
       </c>
       <c r="E108" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B109" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D109">
         <v>20231106</v>
       </c>
       <c r="E109" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B110" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="C110" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D110">
         <v>20231106</v>
       </c>
       <c r="E110" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B111" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D111">
         <v>20231106</v>
       </c>
       <c r="E111" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B112" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D112">
         <v>20231106</v>
       </c>
       <c r="E112" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B113" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D113">
         <v>20231106</v>
       </c>
       <c r="E113" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B114" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D114">
         <v>20231106</v>
       </c>
       <c r="E114" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B115" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D115">
         <v>20231106</v>
       </c>
       <c r="E115" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B116" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D116">
         <v>20231106</v>
       </c>
       <c r="E116" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B117" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C117" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D117">
         <v>20231106</v>
       </c>
       <c r="E117" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B118" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D118">
         <v>20231106</v>
       </c>
       <c r="E118" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C119" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D119">
         <v>20231106</v>
       </c>
       <c r="E119" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B120" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D120">
         <v>20231106</v>
       </c>
       <c r="E120" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B121" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D121">
         <v>20231106</v>
       </c>
       <c r="E121" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B122" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="D122">
         <v>20231106</v>
       </c>
       <c r="E122" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B123" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C123" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D123">
         <v>20231106</v>
       </c>
       <c r="E123" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B124" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C124" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D124">
         <v>20231106</v>
       </c>
       <c r="E124" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B125" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C125" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D125">
         <v>20231106</v>
       </c>
       <c r="E125" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B126" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C126" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D126">
         <v>20231106</v>
       </c>
       <c r="E126" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B127" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C127" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D127">
         <v>20231106</v>
       </c>
       <c r="E127" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B128" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C128" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D128">
         <v>20231106</v>
       </c>
       <c r="E128" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B129" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C129" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D129">
         <v>20231106</v>
       </c>
       <c r="E129" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B130" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C130" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D130">
         <v>20231106</v>
       </c>
       <c r="E130" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B131" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C131" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D131">
         <v>20231106</v>
       </c>
       <c r="E131" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B132" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C132" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D132">
         <v>20231106</v>
       </c>
       <c r="E132" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B133" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C133" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D133">
         <v>20231106</v>
       </c>
       <c r="E133" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B134" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D134">
         <v>20231106</v>
       </c>
       <c r="E134" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B135" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C135" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D135">
         <v>20231106</v>
       </c>
       <c r="E135" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B136" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C136" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D136">
         <v>20231106</v>
       </c>
       <c r="E136" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B137" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C137" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D137">
         <v>20231106</v>
       </c>
       <c r="E137" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B138" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C138" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D138">
         <v>20231106</v>
       </c>
       <c r="E138" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B139" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C139" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D139">
         <v>20231106</v>
       </c>
       <c r="E139" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B140" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C140" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D140">
         <v>20231106</v>
       </c>
       <c r="E140" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B141" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C141" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D141">
         <v>20231106</v>
       </c>
       <c r="E141" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B142" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C142" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D142">
         <v>20231106</v>
       </c>
       <c r="E142" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>